<commit_message>
edit order individual item edit completed
</commit_message>
<xml_diff>
--- a/KatalonProjects/miscData.xlsx
+++ b/KatalonProjects/miscData.xlsx
@@ -372,7 +372,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5448</v>
+        <v>3701</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -380,7 +380,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5449</v>
+        <v>3703</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>

</xml_diff>